<commit_message>
add comments. update deliverables
</commit_message>
<xml_diff>
--- a/deliverables/DTT-Assessment-Hour-Log.xlsx
+++ b/deliverables/DTT-Assessment-Hour-Log.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ca1349bade5a11c9/MS/JOB_HUNT_WEB_DEV/DTT/Assessment/DTT Assessment - Frontend - 2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="346" documentId="8_{49F91033-96F3-7148-A020-201798871A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{26B5561B-6D54-4C76-BA8E-D65271F351E0}"/>
+  <xr:revisionPtr revIDLastSave="397" documentId="8_{49F91033-96F3-7148-A020-201798871A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C20EAF20-17D0-4278-817D-9F99546F3C26}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25800" yWindow="0" windowWidth="25800" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DTT Test Hour Log" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>Subject</t>
   </si>
@@ -85,9 +85,6 @@
     <t>Create header/navbar with links</t>
   </si>
   <si>
-    <t>0.5</t>
-  </si>
-  <si>
     <t>- Create about page and add Read.me file to the project</t>
   </si>
   <si>
@@ -209,6 +206,32 @@
   </si>
   <si>
     <t>- Add media queries for mobile design (max-width: 500px)</t>
+  </si>
+  <si>
+    <t>UI Checks</t>
+  </si>
+  <si>
+    <t>- Fix image in houseDetails to always fit correctly
+- Remove click events from router link to update image in mobile view
+- Create Axios instance in vuex store to avoid repetition on base url and api key on every request
+- Migrate all API calls to vuex store</t>
+  </si>
+  <si>
+    <t>Structure Checks</t>
+  </si>
+  <si>
+    <t>- Fix gargare input to only accept yes or no as options
+- Convert required input fields to type number
+- Fix additional House number to be parsed in the correct input field - Edit house
+- Update form validation for construction year. Don't allow year to be less than the  minimum posible value. Display error accordingly
+- Fix error after creating a new listing. Expect the correct data format for displaying the houseDetail page
+- Add vuex-persistedstate package and configure data to be stored in localstorage so data is not lost on refresh</t>
+  </si>
+  <si>
+    <t>Favorites</t>
+  </si>
+  <si>
+    <t>- Allow the user to like a house (favorites array in vuex sotre) and then be able to filter the houses list by favorites</t>
   </si>
 </sst>
 </file>
@@ -538,6 +561,17 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -549,17 +583,6 @@
     </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="6" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1822,16 +1845,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A18" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21:B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.69921875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.69921875" style="28" customWidth="1"/>
+    <col min="2" max="2" width="10.69921875" style="24" customWidth="1"/>
     <col min="3" max="3" width="8.59765625" style="1" customWidth="1"/>
     <col min="4" max="4" width="43" style="1" customWidth="1"/>
     <col min="5" max="6" width="6.5" style="1" customWidth="1"/>
@@ -1839,28 +1862,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18"/>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
+      <c r="A1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
       <c r="E1" s="9"/>
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="21"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="28"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="18" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="13" t="s">
@@ -1878,14 +1901,14 @@
       <c r="A4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="23">
+      <c r="B4" s="19">
         <v>1</v>
       </c>
       <c r="C4" s="16">
         <v>44961</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="4"/>
@@ -1894,304 +1917,418 @@
       <c r="A5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="23">
+      <c r="B5" s="19">
         <v>1.5</v>
       </c>
       <c r="C5" s="16">
         <v>44961</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="23">
+        <v>27</v>
+      </c>
+      <c r="B6" s="19">
         <v>1</v>
       </c>
       <c r="C6" s="16">
         <v>44961</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" ht="51" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="23">
+        <v>12</v>
+      </c>
+      <c r="B7" s="19">
         <v>1.5</v>
       </c>
       <c r="C7" s="16">
         <v>44961</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="23">
+        <v>28</v>
+      </c>
+      <c r="B8" s="19">
         <v>2</v>
       </c>
       <c r="C8" s="16">
         <v>44962</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" ht="127.5" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="23">
+        <v>13</v>
+      </c>
+      <c r="B9" s="19">
         <v>4</v>
       </c>
       <c r="C9" s="16">
         <v>44962</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E9" s="15"/>
       <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="23">
+        <v>15</v>
+      </c>
+      <c r="B10" s="19">
         <v>3</v>
       </c>
       <c r="C10" s="16">
         <v>44963</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="23">
+        <v>16</v>
+      </c>
+      <c r="B11" s="19">
         <v>2</v>
       </c>
       <c r="C11" s="16">
         <v>44963</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E11" s="15"/>
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="23">
+        <v>17</v>
+      </c>
+      <c r="B12" s="19">
         <v>0.5</v>
       </c>
       <c r="C12" s="16">
         <v>44964</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="23">
+        <v>18</v>
+      </c>
+      <c r="B13" s="19">
         <v>2</v>
       </c>
       <c r="C13" s="16">
         <v>44964</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E13" s="15"/>
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="23">
+        <v>19</v>
+      </c>
+      <c r="B14" s="19">
         <v>1.5</v>
       </c>
       <c r="C14" s="16">
         <v>44964</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E14" s="15"/>
       <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="23">
+        <v>21</v>
+      </c>
+      <c r="B15" s="19">
         <v>1.5</v>
       </c>
       <c r="C15" s="16">
         <v>44964</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E15" s="15"/>
       <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:6" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="23">
+        <v>22</v>
+      </c>
+      <c r="B16" s="19">
         <v>3</v>
       </c>
       <c r="C16" s="16">
         <v>44964</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E16" s="15"/>
       <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" s="23">
+        <v>33</v>
+      </c>
+      <c r="B17" s="19">
         <v>2</v>
       </c>
       <c r="C17" s="16">
         <v>44965</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E17" s="15"/>
       <c r="F17" s="4"/>
     </row>
     <row r="18" spans="1:6" ht="153" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="23">
+        <v>23</v>
+      </c>
+      <c r="B18" s="19">
         <v>5</v>
       </c>
       <c r="C18" s="16">
         <v>44966</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E18" s="15"/>
       <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="23">
+        <v>24</v>
+      </c>
+      <c r="B19" s="19">
         <v>1</v>
       </c>
       <c r="C19" s="16">
         <v>44602</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E19" s="15"/>
       <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" s="23" t="s">
-        <v>10</v>
+        <v>25</v>
+      </c>
+      <c r="B20" s="19">
+        <v>0.5</v>
       </c>
       <c r="C20" s="16">
         <v>44602</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E20" s="15" t="s">
         <v>6</v>
       </c>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="10"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="3"/>
+    <row r="21" spans="1:6" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="19">
+        <v>1.5</v>
+      </c>
+      <c r="C21" s="16">
+        <v>44608</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="15"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="12" t="s">
+    <row r="22" spans="1:6" ht="127.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="19">
+        <v>3</v>
+      </c>
+      <c r="C22" s="16">
+        <v>44609</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" s="15"/>
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="19">
+        <v>2</v>
+      </c>
+      <c r="C23" s="16">
+        <v>44611</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" s="4"/>
+    </row>
+    <row r="24" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A24" s="14"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="4"/>
+    </row>
+    <row r="25" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="4"/>
+    </row>
+    <row r="26" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A26" s="14"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="4"/>
+    </row>
+    <row r="27" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A27" s="14"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="4"/>
+    </row>
+    <row r="28" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A28" s="14"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="4"/>
+    </row>
+    <row r="29" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A29" s="14"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="4"/>
+    </row>
+    <row r="30" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A30" s="14"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="4"/>
+    </row>
+    <row r="31" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A31" s="14"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="4"/>
+    </row>
+    <row r="32" spans="1:6" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="10"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="4"/>
+    </row>
+    <row r="33" spans="1:6" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="25">
-        <f>SUMIF(E4:E20,"&lt;&gt;x",B4:B20)</f>
-        <v>32.5</v>
-      </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="4"/>
-    </row>
-    <row r="23" spans="1:6" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="4"/>
-    </row>
-    <row r="24" spans="1:6" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="4"/>
-    </row>
-    <row r="25" spans="1:6" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="27"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="8"/>
+      <c r="B33" s="21">
+        <f>SUMIF(E4:E31,"&lt;&gt;x",B4:B31)</f>
+        <v>37</v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="4"/>
+    </row>
+    <row r="34" spans="1:6" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="5"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="4"/>
+    </row>
+    <row r="35" spans="1:6" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="5"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="4"/>
+    </row>
+    <row r="36" spans="1:6" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="6"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>